<commit_message>
Updates to AWS code and Figures script
</commit_message>
<xml_diff>
--- a/Aim1/figures/Table1_Additional_Features_v2.xlsx
+++ b/Aim1/figures/Table1_Additional_Features_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/aspen-fire/Aim1/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="361" documentId="8_{6CB627EE-88D2-8042-809D-618E5458D47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3769D6E8-F68D-9641-AB41-E7E9B03EF9F3}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{6CB627EE-88D2-8042-809D-618E5458D47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{488524E7-E80A-8545-86C0-396921D25BF9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{D33BB963-CF9E-8141-9A59-4556936D6419}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{D33BB963-CF9E-8141-9A59-4556936D6419}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -330,7 +330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,14 +380,6 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -472,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -523,17 +515,15 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -560,6 +550,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,9 +575,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -622,7 +615,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -728,7 +721,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -870,7 +863,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -878,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6A9BD-C52E-E74F-A6F1-6A1328C395AA}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B16"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,122 +895,126 @@
       <c r="A2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="22">
-        <v>23957</v>
+      <c r="B2" s="33">
+        <v>26704.926061308</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="22">
-        <v>13421</v>
+      <c r="B3" s="33">
+        <v>15471.821043517</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="22">
-        <v>12991</v>
+      <c r="B4" s="33">
+        <v>14753.3560328289</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="22">
-        <v>7637</v>
+      <c r="B5" s="33">
+        <v>9044.5796044621893</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="22">
-        <v>3537</v>
+      <c r="B6" s="33">
+        <v>4230.1778754854704</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="22">
-        <v>3273</v>
+      <c r="B7" s="33">
+        <v>4101.1956234354602</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="22">
-        <v>2869</v>
+      <c r="B8" s="33">
+        <v>3446.0839882977598</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="22">
-        <v>1016</v>
+        <v>89</v>
+      </c>
+      <c r="B9" s="33">
+        <v>1328.90838049127</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="22">
-        <v>896</v>
+        <v>87</v>
+      </c>
+      <c r="B10" s="33">
+        <v>1324.51686155888</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="22">
-        <v>808</v>
+        <v>81</v>
+      </c>
+      <c r="B11" s="33">
+        <v>1249.4624102707</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="22">
-        <v>716</v>
+      <c r="B12" s="33">
+        <v>993.23068377766594</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="22">
-        <v>669</v>
+      <c r="B13" s="33">
+        <v>984.57812598711905</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="22">
-        <v>624</v>
+      <c r="B14" s="33">
+        <v>880.67861410738305</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="24">
-        <v>617</v>
+      <c r="B15" s="35">
+        <v>874.75695856999198</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="34">
         <f>SUM(B2:B15)</f>
-        <v>73031</v>
-      </c>
+        <v>85388.272264097803</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="22"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B15">
@@ -1063,7 +1060,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="26" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1075,12 +1072,12 @@
       <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="26" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="16" t="s">
         <v>20</v>
       </c>
@@ -1090,10 +1087,10 @@
       <c r="D3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="29"/>
+      <c r="E3" s="27"/>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1105,12 +1102,12 @@
       <c r="D4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="28" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1120,10 +1117,10 @@
       <c r="D5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1133,10 +1130,10 @@
       <c r="D6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1146,10 +1143,10 @@
       <c r="D7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1159,10 +1156,10 @@
       <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1172,10 +1169,10 @@
       <c r="D9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1185,10 +1182,10 @@
       <c r="D10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1198,10 +1195,10 @@
       <c r="D11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="29"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="31"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1211,10 +1208,10 @@
       <c r="D12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="29"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1224,16 +1221,16 @@
       <c r="D13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="1:5" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1313,7 +1310,7 @@
       <c r="D2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="30" t="s">
         <v>53</v>
       </c>
       <c r="F2" s="11"/>
@@ -1331,7 +1328,7 @@
       <c r="D3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="33"/>
+      <c r="E3" s="31"/>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1347,7 +1344,7 @@
       <c r="D4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="31"/>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1363,7 +1360,7 @@
       <c r="D5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="32"/>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,7 +1376,7 @@
       <c r="D6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="30" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="11"/>
@@ -1397,7 +1394,7 @@
       <c r="D7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="33"/>
+      <c r="E7" s="31"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1410,7 @@
       <c r="D8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1429,7 +1426,7 @@
       <c r="D9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="33"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1445,7 +1442,7 @@
       <c r="D10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="33"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1461,7 +1458,7 @@
       <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to VIIRS cloud-processing workflow
</commit_message>
<xml_diff>
--- a/Aim1/figures/Table1_Additional_Features_v2.xlsx
+++ b/Aim1/figures/Table1_Additional_Features_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6270a8f4b8f62cae/mcook/aspen-fire/Aim1/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="371" documentId="8_{6CB627EE-88D2-8042-809D-618E5458D47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{488524E7-E80A-8545-86C0-396921D25BF9}"/>
+  <xr:revisionPtr revIDLastSave="373" documentId="8_{6CB627EE-88D2-8042-809D-618E5458D47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{194F204F-4C06-E241-AA64-69E5E01C39DA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{D33BB963-CF9E-8141-9A59-4556936D6419}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="2" xr2:uid="{D33BB963-CF9E-8141-9A59-4556936D6419}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="4" r:id="rId1"/>
@@ -526,33 +526,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,14 +570,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -615,7 +611,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -721,7 +717,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -863,7 +859,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -873,7 +869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C6A9BD-C52E-E74F-A6F1-6A1328C395AA}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -895,7 +891,7 @@
       <c r="A2" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="25">
         <v>26704.926061308</v>
       </c>
     </row>
@@ -903,7 +899,7 @@
       <c r="A3" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="25">
         <v>15471.821043517</v>
       </c>
     </row>
@@ -911,7 +907,7 @@
       <c r="A4" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="25">
         <v>14753.3560328289</v>
       </c>
     </row>
@@ -919,7 +915,7 @@
       <c r="A5" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="25">
         <v>9044.5796044621893</v>
       </c>
     </row>
@@ -927,7 +923,7 @@
       <c r="A6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="25">
         <v>4230.1778754854704</v>
       </c>
     </row>
@@ -935,7 +931,7 @@
       <c r="A7" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="25">
         <v>4101.1956234354602</v>
       </c>
     </row>
@@ -943,7 +939,7 @@
       <c r="A8" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="25">
         <v>3446.0839882977598</v>
       </c>
     </row>
@@ -951,7 +947,7 @@
       <c r="A9" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="25">
         <v>1328.90838049127</v>
       </c>
     </row>
@@ -959,7 +955,7 @@
       <c r="A10" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="25">
         <v>1324.51686155888</v>
       </c>
     </row>
@@ -967,7 +963,7 @@
       <c r="A11" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="25">
         <v>1249.4624102707</v>
       </c>
     </row>
@@ -975,7 +971,7 @@
       <c r="A12" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="25">
         <v>993.23068377766594</v>
       </c>
     </row>
@@ -983,7 +979,7 @@
       <c r="A13" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="25">
         <v>984.57812598711905</v>
       </c>
     </row>
@@ -991,7 +987,7 @@
       <c r="A14" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="25">
         <v>880.67861410738305</v>
       </c>
     </row>
@@ -999,7 +995,7 @@
       <c r="A15" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="27">
         <v>874.75695856999198</v>
       </c>
     </row>
@@ -1007,7 +1003,7 @@
       <c r="A16" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="26">
         <f>SUM(B2:B15)</f>
         <v>85388.272264097803</v>
       </c>
@@ -1060,7 +1056,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="29" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1072,12 +1068,12 @@
       <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="29" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="16" t="s">
         <v>20</v>
       </c>
@@ -1087,10 +1083,10 @@
       <c r="D3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="27"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1102,12 +1098,12 @@
       <c r="D4" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1117,10 +1113,10 @@
       <c r="D5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1130,10 +1126,10 @@
       <c r="D6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1143,10 +1139,10 @@
       <c r="D7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1156,10 +1152,10 @@
       <c r="D8" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1169,10 +1165,10 @@
       <c r="D9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1182,10 +1178,10 @@
       <c r="D10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1195,10 +1191,10 @@
       <c r="D11" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1208,10 +1204,10 @@
       <c r="D12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1221,16 +1217,16 @@
       <c r="D13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="32"/>
     </row>
     <row r="14" spans="1:5" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1263,8 +1259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6AFAC0-8994-8D47-A8D9-24432B6CA267}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1268,7 @@
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
   </cols>
@@ -1310,7 +1306,7 @@
       <c r="D2" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>53</v>
       </c>
       <c r="F2" s="11"/>
@@ -1328,7 +1324,7 @@
       <c r="D3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1344,7 +1340,7 @@
       <c r="D4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -1360,7 +1356,7 @@
       <c r="D5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1376,7 +1372,7 @@
       <c r="D6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="33" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="11"/>
@@ -1394,7 +1390,7 @@
       <c r="D7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1410,7 +1406,7 @@
       <c r="D8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1426,7 +1422,7 @@
       <c r="D9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1442,7 +1438,7 @@
       <c r="D10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="31"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
@@ -1458,7 +1454,7 @@
       <c r="D11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="31"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="11"/>
     </row>
   </sheetData>
@@ -1468,6 +1464,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>